<commit_message>
Add visited column to ballpark data
</commit_message>
<xml_diff>
--- a/public/data/Ballparks.xlsx
+++ b/public/data/Ballparks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikmd\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E924B023-CED9-4C04-86A5-CED95FFA524F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E49D3A6-5B3B-42AE-BAB6-E00ACB549AD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="33946" windowHeight="22096" xr2:uid="{64A02C90-724C-40E9-82C3-F967BBB77E6F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="492">
   <si>
     <t>WI</t>
   </si>
@@ -1479,12 +1479,6 @@
     <t>VenueCountry</t>
   </si>
   <si>
-    <t>VenueLatitude</t>
-  </si>
-  <si>
-    <t>VenueLongitude</t>
-  </si>
-  <si>
     <t>VenueUrl</t>
   </si>
   <si>
@@ -1504,6 +1498,15 @@
   </si>
   <si>
     <t>https://www.mlb.com/astros/ballpark</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Visited</t>
   </si>
 </sst>
 </file>
@@ -1547,9 +1550,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1864,10 +1868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E3A356-E4B9-401F-9581-53C9D178E23F}">
-  <dimension ref="A1:S61"/>
+  <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1893,7 +1897,7 @@
     <col min="21" max="21" width="95.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>465</v>
       </c>
@@ -1943,16 +1947,19 @@
         <v>481</v>
       </c>
       <c r="Q1" t="s">
+        <v>489</v>
+      </c>
+      <c r="R1" t="s">
+        <v>490</v>
+      </c>
+      <c r="S1" t="s">
         <v>482</v>
       </c>
-      <c r="R1" t="s">
-        <v>483</v>
-      </c>
-      <c r="S1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T1" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1233</v>
       </c>
@@ -2010,8 +2017,11 @@
       <c r="S2" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1234</v>
       </c>
@@ -2069,8 +2079,11 @@
       <c r="S3" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1235</v>
       </c>
@@ -2128,8 +2141,11 @@
       <c r="S4" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1236</v>
       </c>
@@ -2187,8 +2203,11 @@
       <c r="S5" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1237</v>
       </c>
@@ -2246,8 +2265,11 @@
       <c r="S6" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1238</v>
       </c>
@@ -2305,8 +2327,11 @@
       <c r="S7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1239</v>
       </c>
@@ -2364,8 +2389,11 @@
       <c r="S8" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>1240</v>
       </c>
@@ -2423,8 +2451,11 @@
       <c r="S9" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>1241</v>
       </c>
@@ -2482,8 +2513,11 @@
       <c r="S10" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>1242</v>
       </c>
@@ -2541,8 +2575,11 @@
       <c r="S11" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1243</v>
       </c>
@@ -2600,8 +2637,11 @@
       <c r="S12" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1244</v>
       </c>
@@ -2659,8 +2699,11 @@
       <c r="S13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1245</v>
       </c>
@@ -2715,8 +2758,11 @@
       <c r="R14">
         <v>-76.165369999999896</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>1246</v>
       </c>
@@ -2774,8 +2820,11 @@
       <c r="S15" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1247</v>
       </c>
@@ -2833,8 +2882,11 @@
       <c r="S16" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>1249</v>
       </c>
@@ -2892,8 +2944,11 @@
       <c r="S17" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>1250</v>
       </c>
@@ -2951,8 +3006,11 @@
       <c r="S18" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>1251</v>
       </c>
@@ -3010,8 +3068,11 @@
       <c r="S19" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>1252</v>
       </c>
@@ -3069,8 +3130,11 @@
       <c r="S20" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>1253</v>
       </c>
@@ -3128,8 +3192,11 @@
       <c r="S21" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>1254</v>
       </c>
@@ -3187,8 +3254,11 @@
       <c r="S22" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>1255</v>
       </c>
@@ -3243,8 +3313,11 @@
       <c r="R23">
         <v>-90.199712000000005</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>1256</v>
       </c>
@@ -3302,8 +3375,11 @@
       <c r="S24" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>1257</v>
       </c>
@@ -3361,8 +3437,11 @@
       <c r="S25" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>1258</v>
       </c>
@@ -3420,8 +3499,11 @@
       <c r="S26" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>1259</v>
       </c>
@@ -3479,8 +3561,11 @@
       <c r="S27" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>1260</v>
       </c>
@@ -3538,8 +3623,11 @@
       <c r="S28" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>1261</v>
       </c>
@@ -3597,8 +3685,11 @@
       <c r="S29" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>1329</v>
       </c>
@@ -3656,8 +3747,11 @@
       <c r="S30" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>1262</v>
       </c>
@@ -3715,8 +3809,11 @@
       <c r="S31" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>232</v>
       </c>
@@ -3771,8 +3868,11 @@
       <c r="S32" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>225</v>
       </c>
@@ -3827,8 +3927,11 @@
       <c r="S33" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>241</v>
       </c>
@@ -3883,8 +3986,11 @@
       <c r="S34" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>227</v>
       </c>
@@ -3939,8 +4045,11 @@
       <c r="S35" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>222</v>
       </c>
@@ -3995,8 +4104,11 @@
       <c r="S36" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>230</v>
       </c>
@@ -4049,10 +4161,13 @@
         <v>-95.355540000000005</v>
       </c>
       <c r="S37" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.45">
+        <v>488</v>
+      </c>
+      <c r="T37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>228</v>
       </c>
@@ -4105,10 +4220,13 @@
         <v>-94.480429930999904</v>
       </c>
       <c r="S38" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.45">
+        <v>487</v>
+      </c>
+      <c r="T38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>219</v>
       </c>
@@ -4161,10 +4279,13 @@
         <v>-117.88271</v>
       </c>
       <c r="S39" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.45">
+        <v>486</v>
+      </c>
+      <c r="T39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>245</v>
       </c>
@@ -4219,8 +4340,11 @@
       <c r="S40" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>243</v>
       </c>
@@ -4275,8 +4399,11 @@
       <c r="S41" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>370</v>
       </c>
@@ -4329,10 +4456,13 @@
         <v>-122.20062</v>
       </c>
       <c r="S42" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.45">
+        <v>485</v>
+      </c>
+      <c r="T42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>236</v>
       </c>
@@ -4387,8 +4517,11 @@
       <c r="S43" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>239</v>
       </c>
@@ -4443,8 +4576,11 @@
       <c r="S44" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>238</v>
       </c>
@@ -4499,8 +4635,11 @@
       <c r="S45" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>247</v>
       </c>
@@ -4555,8 +4694,11 @@
       <c r="S46" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>220</v>
       </c>
@@ -4609,10 +4751,13 @@
         <v>-112.06680131500001</v>
       </c>
       <c r="S47" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.45">
+        <v>484</v>
+      </c>
+      <c r="T47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>1293</v>
       </c>
@@ -4667,8 +4812,11 @@
       <c r="S48" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>242</v>
       </c>
@@ -4723,8 +4871,11 @@
       <c r="S49" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>226</v>
       </c>
@@ -4779,8 +4930,11 @@
       <c r="S50" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>223</v>
       </c>
@@ -4835,8 +4989,11 @@
       <c r="S51" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>224</v>
       </c>
@@ -4889,10 +5046,13 @@
         <v>-118.23994999999999</v>
       </c>
       <c r="S52" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.45">
+        <v>483</v>
+      </c>
+      <c r="T52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>248</v>
       </c>
@@ -4947,8 +5107,11 @@
       <c r="S53" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>229</v>
       </c>
@@ -5003,8 +5166,11 @@
       <c r="S54" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>237</v>
       </c>
@@ -5059,8 +5225,11 @@
       <c r="S55" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>221</v>
       </c>
@@ -5115,8 +5284,11 @@
       <c r="S56" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>235</v>
       </c>
@@ -5171,8 +5343,11 @@
       <c r="S57" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>231</v>
       </c>
@@ -5227,8 +5402,11 @@
       <c r="S58" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>234</v>
       </c>
@@ -5283,8 +5461,11 @@
       <c r="S59" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>233</v>
       </c>
@@ -5339,8 +5520,11 @@
       <c r="S60" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>244</v>
       </c>
@@ -5394,6 +5578,9 @@
       </c>
       <c r="S61" t="s">
         <v>78</v>
+      </c>
+      <c r="T61" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>